<commit_message>
changes so i can work a little this weekend
</commit_message>
<xml_diff>
--- a/hst/galaxydata.xlsx
+++ b/hst/galaxydata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23540" yWindow="17960" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="22400" yWindow="9580" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>J1219+0336</t>
   </si>
   <si>
-    <t>J1341-0321</t>
-  </si>
-  <si>
     <t>J1506+5402</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>J2140+1209</t>
+  </si>
+  <si>
+    <t>J1341+0321</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
         <v>0.65800000000000003</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>0.60799999999999998</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>0.40200000000000002</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>0.44900000000000001</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2">
         <v>0.72799999999999998</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2">
         <v>0.752</v>

</xml_diff>